<commit_message>
Fix wrong test  filter and template
</commit_message>
<xml_diff>
--- a/subscription_report/ppu_subscriptions_by_product_month/template.xlsx
+++ b/subscription_report/ppu_subscriptions_by_product_month/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\CheckPoint Reseller Dashboard\CheckPointCustomReports\subscription_report\ppu_subscriptions_by_product_month\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\ConnectCustomSubscriptionReport\subscription_report\ppu_subscriptions_by_product_month\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DDBFA4-3E0B-4FD6-BEA8-7D38A8CE53DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250C05A3-9EAE-407D-974A-1C00D6CFF20F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Service Description in the partner and customer invoice</t>
+          <t>Service Description for the reseller and customer invoice</t>
         </r>
       </text>
     </comment>
@@ -64,7 +64,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Subscription Item MPN</t>
+          <t>Item MPN with quantity to report</t>
         </r>
       </text>
     </comment>
@@ -77,7 +77,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Devices/users quantity</t>
+          <t>Measured quantity</t>
         </r>
       </text>
     </comment>
@@ -116,7 +116,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Subscription Activation Key value</t>
+          <t>Subscription Parameter Id value</t>
         </r>
       </text>
     </comment>
@@ -677,7 +677,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -857,6 +857,11 @@
   </sheetData>
   <autoFilter ref="A1:Q2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D23" xr:uid="{00000000-0002-0000-0100-000001000000}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <customProperties>
@@ -865,19 +870,13 @@
   <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>categories!$A$2:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>O2:O25</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D23</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -885,6 +884,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100316493EAEB2DBF409C59D3E28FDCE060" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="021ace4200c022706e53606a445e80e6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="405bfd55-4c25-4c93-a26b-cf6165de5e2d" xmlns:ns4="a7b43b79-810c-4ee8-933c-299c110e8a84" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="af83b860b95128a706bfadeedaaf1c4a" ns3:_="" ns4:_="">
     <xsd:import namespace="405bfd55-4c25-4c93-a26b-cf6165de5e2d"/>
@@ -1101,15 +1109,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1117,6 +1116,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C88A616-90DB-4CFA-8A02-8983945A79BF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77CE1762-47B1-43FA-A733-3535CE915398}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1135,14 +1142,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C88A616-90DB-4CFA-8A02-8983945A79BF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FB93A58-0C18-4BE7-978A-738EC8E406EB}">
   <ds:schemaRefs>

</xml_diff>